<commit_message>
MaJ Gantt, redéfinition des pôles d'activités
</commit_message>
<xml_diff>
--- a/GanttPRO_Semaine.xlsx
+++ b/GanttPRO_Semaine.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Gantt!$A$1:$AG$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Gantt!$A$1:$AG$38</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Gantt!$A$1:$AG$38</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t xml:space="preserve">PRO</t>
   </si>
@@ -34,7 +35,7 @@
         <b val="true"/>
         <sz val="22"/>
         <rFont val="Century Gothic"/>
-        <family val="0"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Planification du projet
@@ -44,7 +45,7 @@
       <rPr>
         <sz val="14"/>
         <rFont val="Century Gothic"/>
-        <family val="0"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Découpage par demi-semaine</t>
@@ -162,6 +163,9 @@
     <t xml:space="preserve">Conception de la Base de donnée</t>
   </si>
   <si>
+    <t xml:space="preserve">END</t>
+  </si>
+  <si>
     <t xml:space="preserve">Extraction, traitement du fichier ICS</t>
   </si>
   <si>
@@ -171,13 +175,25 @@
     <t xml:space="preserve">Implémentation et tests des requetes</t>
   </si>
   <si>
+    <t xml:space="preserve">A+D</t>
+  </si>
+  <si>
     <t xml:space="preserve">Client-server connexion et communication</t>
   </si>
   <si>
-    <t xml:space="preserve">Heuristique calcul – Traitement de la réponse</t>
+    <t xml:space="preserve">Heuristique calcul</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> – Traitement de la réponse</t>
   </si>
   <si>
     <t xml:space="preserve">Interface Graphique – Mockup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implémentation serveur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retour client</t>
   </si>
   <si>
     <t xml:space="preserve">Procédure de tests</t>
@@ -210,7 +226,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -236,7 +252,7 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -256,25 +272,11 @@
       <b val="true"/>
       <sz val="22"/>
       <name val="Century Gothic"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
-      <name val="Century Gothic"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="16"/>
-      <name val="Century Gothic"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
       <name val="Century Gothic"/>
       <family val="2"/>
       <charset val="1"/>
@@ -287,9 +289,16 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Century Gothic"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -313,22 +322,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="16"/>
-      <name val="Century Gothic"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -564,7 +562,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -597,7 +595,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -617,31 +615,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -649,11 +647,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -661,95 +703,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="13" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="10" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="10" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="13" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="13" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="13" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="14" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="12" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="13" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="13" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="14" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="9" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -761,7 +755,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -831,17 +825,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AJ1048576"/>
+  <dimension ref="A1:AJ38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P29" activeCellId="0" sqref="P29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O27" activeCellId="0" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="51.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="2" style="2" width="7.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="10.49"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.9162790697674"/>
+    <col collapsed="false" hidden="false" max="33" min="2" style="2" width="7.75348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="10.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1397,7 +1391,7 @@
       <c r="AG12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="28"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -1430,47 +1424,47 @@
       <c r="AE13" s="17"/>
       <c r="AF13" s="17"/>
       <c r="AG13" s="19"/>
-      <c r="AI13" s="29"/>
+      <c r="AI13" s="28"/>
       <c r="AJ13" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="31"/>
-      <c r="Z14" s="31"/>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="31"/>
-      <c r="AC14" s="31"/>
-      <c r="AD14" s="31"/>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31"/>
-      <c r="AG14" s="32"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="30"/>
+      <c r="AA14" s="30"/>
+      <c r="AB14" s="30"/>
+      <c r="AC14" s="30"/>
+      <c r="AD14" s="30"/>
+      <c r="AE14" s="30"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
@@ -1508,13 +1502,13 @@
       <c r="AE15" s="17"/>
       <c r="AF15" s="17"/>
       <c r="AG15" s="19"/>
-      <c r="AI15" s="33"/>
+      <c r="AI15" s="32"/>
       <c r="AJ15" s="0" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="17"/>
@@ -1551,7 +1545,7 @@
       <c r="AG16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -1584,47 +1578,47 @@
       <c r="AE17" s="17"/>
       <c r="AF17" s="17"/>
       <c r="AG17" s="19"/>
-      <c r="AI17" s="34"/>
-      <c r="AJ17" s="35" t="s">
+      <c r="AI17" s="33"/>
+      <c r="AJ17" s="34" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="37"/>
-      <c r="AA18" s="37"/>
-      <c r="AB18" s="37"/>
-      <c r="AC18" s="37"/>
-      <c r="AD18" s="37"/>
-      <c r="AE18" s="37"/>
-      <c r="AF18" s="37"/>
-      <c r="AG18" s="38"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36"/>
+      <c r="Z18" s="36"/>
+      <c r="AA18" s="36"/>
+      <c r="AB18" s="36"/>
+      <c r="AC18" s="36"/>
+      <c r="AD18" s="36"/>
+      <c r="AE18" s="36"/>
+      <c r="AF18" s="36"/>
+      <c r="AG18" s="37"/>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
@@ -1639,9 +1633,11 @@
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="17"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
@@ -1664,8 +1660,8 @@
       <c r="AG19" s="19"/>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="41" t="s">
-        <v>39</v>
+      <c r="A20" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -1676,11 +1672,13 @@
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="P20" s="17"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
@@ -1702,7 +1700,7 @@
     </row>
     <row r="21" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1713,12 +1711,14 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="Q21" s="17"/>
       <c r="R21" s="17"/>
       <c r="S21" s="17"/>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="22" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1752,9 +1752,11 @@
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="17"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="P22" s="17"/>
       <c r="Q22" s="17"/>
       <c r="R22" s="17"/>
@@ -1775,8 +1777,8 @@
       <c r="AG22" s="19"/>
     </row>
     <row r="23" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28" t="s">
-        <v>42</v>
+      <c r="A23" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1787,10 +1789,10 @@
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="17"/>
@@ -1812,8 +1814,8 @@
       <c r="AG23" s="19"/>
     </row>
     <row r="24" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28" t="s">
-        <v>43</v>
+      <c r="A24" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -1824,11 +1826,11 @@
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="17"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="17"/>
       <c r="R24" s="17"/>
@@ -1849,8 +1851,8 @@
       <c r="AG24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28" t="s">
-        <v>44</v>
+      <c r="A25" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -1861,11 +1863,11 @@
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="17"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="40"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="17"/>
       <c r="R25" s="17"/>
@@ -1886,7 +1888,9 @@
       <c r="AG25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28"/>
+      <c r="A26" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -1896,11 +1900,11 @@
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="45"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="17"/>
       <c r="R26" s="17"/>
@@ -1921,7 +1925,9 @@
       <c r="AG26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28"/>
+      <c r="A27" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -1931,11 +1937,11 @@
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="43"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
@@ -1956,7 +1962,9 @@
       <c r="AG27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="28"/>
+      <c r="A28" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -1970,7 +1978,7 @@
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
+      <c r="O28" s="38"/>
       <c r="P28" s="17"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="17"/>
@@ -1991,46 +1999,42 @@
       <c r="AG28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
-      <c r="V29" s="14"/>
-      <c r="W29" s="14"/>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="14"/>
-      <c r="Z29" s="14"/>
-      <c r="AA29" s="14"/>
-      <c r="AB29" s="14"/>
-      <c r="AC29" s="14"/>
-      <c r="AD29" s="14"/>
-      <c r="AE29" s="14"/>
-      <c r="AF29" s="14"/>
-      <c r="AG29" s="15"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+      <c r="Y29" s="17"/>
+      <c r="Z29" s="17"/>
+      <c r="AA29" s="17"/>
+      <c r="AB29" s="17"/>
+      <c r="AC29" s="17"/>
+      <c r="AD29" s="17"/>
+      <c r="AE29" s="17"/>
+      <c r="AF29" s="17"/>
+      <c r="AG29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16" t="s">
-        <v>46</v>
-      </c>
+      <c r="A30" s="16"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -2065,81 +2069,81 @@
       <c r="AG30" s="19"/>
     </row>
     <row r="31" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="28"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="17"/>
-      <c r="U31" s="17"/>
-      <c r="V31" s="17"/>
-      <c r="W31" s="17"/>
-      <c r="X31" s="17"/>
-      <c r="Y31" s="17"/>
-      <c r="Z31" s="17"/>
-      <c r="AA31" s="17"/>
-      <c r="AB31" s="17"/>
-      <c r="AC31" s="17"/>
-      <c r="AD31" s="17"/>
-      <c r="AE31" s="17"/>
-      <c r="AF31" s="17"/>
-      <c r="AG31" s="19"/>
+      <c r="A31" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="14"/>
+      <c r="AB31" s="14"/>
+      <c r="AC31" s="14"/>
+      <c r="AD31" s="14"/>
+      <c r="AE31" s="14"/>
+      <c r="AF31" s="14"/>
+      <c r="AG31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="25"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="25"/>
-      <c r="S32" s="25"/>
-      <c r="T32" s="25"/>
-      <c r="U32" s="25"/>
-      <c r="V32" s="25"/>
-      <c r="W32" s="25"/>
-      <c r="X32" s="25"/>
-      <c r="Y32" s="25"/>
-      <c r="Z32" s="25"/>
-      <c r="AA32" s="25"/>
-      <c r="AB32" s="25"/>
-      <c r="AC32" s="25"/>
-      <c r="AD32" s="25"/>
-      <c r="AE32" s="25"/>
-      <c r="AF32" s="25"/>
-      <c r="AG32" s="26"/>
+      <c r="A32" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="17"/>
+      <c r="AB32" s="17"/>
+      <c r="AC32" s="17"/>
+      <c r="AD32" s="17"/>
+      <c r="AE32" s="17"/>
+      <c r="AF32" s="17"/>
+      <c r="AG32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16" t="s">
-        <v>48</v>
-      </c>
+      <c r="A33" s="16"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -2174,45 +2178,45 @@
       <c r="AG33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="17"/>
-      <c r="S34" s="17"/>
-      <c r="T34" s="17"/>
-      <c r="U34" s="17"/>
-      <c r="V34" s="17"/>
-      <c r="W34" s="17"/>
-      <c r="X34" s="17"/>
-      <c r="Y34" s="17"/>
-      <c r="Z34" s="17"/>
-      <c r="AA34" s="17"/>
-      <c r="AB34" s="17"/>
-      <c r="AC34" s="17"/>
-      <c r="AD34" s="17"/>
-      <c r="AE34" s="17"/>
-      <c r="AF34" s="17"/>
-      <c r="AG34" s="19"/>
-    </row>
-    <row r="35" customFormat="false" ht="20.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="25"/>
+      <c r="S34" s="25"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="25"/>
+      <c r="V34" s="25"/>
+      <c r="W34" s="25"/>
+      <c r="X34" s="25"/>
+      <c r="Y34" s="25"/>
+      <c r="Z34" s="25"/>
+      <c r="AA34" s="25"/>
+      <c r="AB34" s="25"/>
+      <c r="AC34" s="25"/>
+      <c r="AD34" s="25"/>
+      <c r="AE34" s="25"/>
+      <c r="AF34" s="25"/>
+      <c r="AG34" s="26"/>
+    </row>
+    <row r="35" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -2247,9 +2251,9 @@
       <c r="AF35" s="17"/>
       <c r="AG35" s="19"/>
     </row>
-    <row r="36" customFormat="false" ht="20.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -2284,7 +2288,80 @@
       <c r="AF36" s="17"/>
       <c r="AG36" s="19"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="20.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17"/>
+      <c r="Y37" s="17"/>
+      <c r="Z37" s="17"/>
+      <c r="AA37" s="17"/>
+      <c r="AB37" s="17"/>
+      <c r="AC37" s="17"/>
+      <c r="AD37" s="17"/>
+      <c r="AE37" s="17"/>
+      <c r="AF37" s="17"/>
+      <c r="AG37" s="19"/>
+    </row>
+    <row r="38" customFormat="false" ht="20.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="17"/>
+      <c r="X38" s="17"/>
+      <c r="Y38" s="17"/>
+      <c r="Z38" s="17"/>
+      <c r="AA38" s="17"/>
+      <c r="AB38" s="17"/>
+      <c r="AC38" s="17"/>
+      <c r="AD38" s="17"/>
+      <c r="AE38" s="17"/>
+      <c r="AF38" s="17"/>
+      <c r="AG38" s="19"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="A1:AG1"/>
@@ -2308,7 +2385,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.590277777777778" right="0.590277777777778" top="2.16527777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="2" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="2" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2323,18 +2400,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.36"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.61395348837209"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
work slices till sunday 13.05
</commit_message>
<xml_diff>
--- a/GanttPRO_Semaine.xlsx
+++ b/GanttPRO_Semaine.xlsx
@@ -12,8 +12,9 @@
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Gantt!$A$1:$AG$38</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Gantt!$A$1:$AG$38</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Gantt!$A$1:$AG$44</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Gantt!$A$1:$AG$44</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Gantt!$A$1:$AG$44</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t xml:space="preserve">PRO</t>
   </si>
@@ -166,6 +167,9 @@
     <t xml:space="preserve">END</t>
   </si>
   <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
     <t xml:space="preserve">Extraction, traitement du fichier ICS</t>
   </si>
   <si>
@@ -190,10 +194,40 @@
     <t xml:space="preserve">Interface Graphique – Mockup</t>
   </si>
   <si>
+    <t xml:space="preserve">Interface Graphique – Implémentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interface Graphique – Extraction données</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implémentation serveur</t>
   </si>
   <si>
-    <t xml:space="preserve">Retour client</t>
+    <t xml:space="preserve">NOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implémentation (+ tests) BDD-parsing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Présentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implémentation GUI-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implémentation gestion data coté client</t>
   </si>
   <si>
     <t xml:space="preserve">Procédure de tests</t>
@@ -209,9 +243,6 @@
   </si>
   <si>
     <t xml:space="preserve">Manuel utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Présentation</t>
   </si>
   <si>
     <t xml:space="preserve">Réunion de groupe</t>
@@ -329,7 +360,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +437,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC6D9F1"/>
         <bgColor rgb="FFE6E0EC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
     <fill>
@@ -562,7 +599,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -723,28 +760,40 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="15" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="9" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="14" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -825,17 +874,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AJ38"/>
+  <dimension ref="A1:AJ44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O27" activeCellId="0" sqref="O27"/>
+      <selection pane="topLeft" activeCell="V33" activeCellId="0" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.9162790697674"/>
-    <col collapsed="false" hidden="false" max="33" min="2" style="2" width="7.75348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.3953488372093"/>
+    <col collapsed="false" hidden="false" max="33" min="2" style="2" width="7.87441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1658,10 +1707,14 @@
       <c r="AE19" s="17"/>
       <c r="AF19" s="17"/>
       <c r="AG19" s="19"/>
+      <c r="AI19" s="40"/>
+      <c r="AJ19" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -1672,10 +1725,10 @@
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
       <c r="O20" s="17" t="s">
         <v>39</v>
       </c>
@@ -1700,7 +1753,7 @@
     </row>
     <row r="21" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1711,11 +1764,11 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
-      <c r="K21" s="40"/>
+      <c r="K21" s="41"/>
       <c r="L21" s="38"/>
-      <c r="M21" s="41"/>
+      <c r="M21" s="42"/>
       <c r="N21" s="38"/>
-      <c r="O21" s="41"/>
+      <c r="O21" s="42"/>
       <c r="P21" s="17" t="s">
         <v>39</v>
       </c>
@@ -1739,7 +1792,7 @@
     </row>
     <row r="22" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1752,18 +1805,32 @@
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
       <c r="O22" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="17"/>
-      <c r="V22" s="17"/>
+        <v>44</v>
+      </c>
+      <c r="P22" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q22" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="R22" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="S22" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="T22" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="U22" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="V22" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="W22" s="17"/>
       <c r="X22" s="17"/>
       <c r="Y22" s="17"/>
@@ -1778,7 +1845,7 @@
     </row>
     <row r="23" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1789,11 +1856,13 @@
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="17"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="P23" s="17"/>
       <c r="Q23" s="17"/>
       <c r="R23" s="17"/>
@@ -1815,7 +1884,7 @@
     </row>
     <row r="24" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -1826,19 +1895,19 @@
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="17"/>
-      <c r="V24" s="17"/>
-      <c r="W24" s="17"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="41"/>
+      <c r="S24" s="43"/>
+      <c r="T24" s="41"/>
+      <c r="U24" s="43"/>
+      <c r="V24" s="41"/>
+      <c r="W24" s="43"/>
       <c r="X24" s="17"/>
       <c r="Y24" s="17"/>
       <c r="Z24" s="17"/>
@@ -1852,7 +1921,7 @@
     </row>
     <row r="25" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -1863,13 +1932,15 @@
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="R25" s="17"/>
       <c r="S25" s="17"/>
       <c r="T25" s="17"/>
@@ -1889,7 +1960,7 @@
     </row>
     <row r="26" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -1926,7 +1997,7 @@
     </row>
     <row r="27" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -1937,18 +2008,20 @@
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="17"/>
-      <c r="V27" s="17"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="45"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="45"/>
+      <c r="V27" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="W27" s="17"/>
       <c r="X27" s="17"/>
       <c r="Y27" s="17"/>
@@ -1963,7 +2036,7 @@
     </row>
     <row r="28" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -1974,17 +2047,17 @@
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="38"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="17"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="45"/>
+      <c r="U28" s="42"/>
       <c r="V28" s="17"/>
       <c r="W28" s="17"/>
       <c r="X28" s="17"/>
@@ -1999,7 +2072,9 @@
       <c r="AG28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16"/>
+      <c r="A29" s="16" t="s">
+        <v>51</v>
+      </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -2013,14 +2088,24 @@
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17"/>
-      <c r="U29" s="17"/>
-      <c r="V29" s="17"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q29" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="S29" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="T29" s="44"/>
+      <c r="U29" s="44"/>
+      <c r="V29" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="W29" s="17"/>
       <c r="X29" s="17"/>
       <c r="Y29" s="17"/>
@@ -2034,7 +2119,9 @@
       <c r="AG29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16"/>
+      <c r="A30" s="16" t="s">
+        <v>54</v>
+      </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -2048,13 +2135,13 @@
       <c r="L30" s="17"/>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="17"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="41"/>
+      <c r="T30" s="38"/>
+      <c r="U30" s="41"/>
       <c r="V30" s="17"/>
       <c r="W30" s="17"/>
       <c r="X30" s="17"/>
@@ -2069,45 +2156,49 @@
       <c r="AG30" s="19"/>
     </row>
     <row r="31" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
-      <c r="U31" s="14"/>
-      <c r="V31" s="14"/>
-      <c r="W31" s="14"/>
-      <c r="X31" s="14"/>
-      <c r="Y31" s="14"/>
-      <c r="Z31" s="14"/>
-      <c r="AA31" s="14"/>
-      <c r="AB31" s="14"/>
-      <c r="AC31" s="14"/>
-      <c r="AD31" s="14"/>
-      <c r="AE31" s="14"/>
-      <c r="AF31" s="14"/>
-      <c r="AG31" s="15"/>
+      <c r="A31" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="P31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+      <c r="AA31" s="17"/>
+      <c r="AB31" s="17"/>
+      <c r="AC31" s="17"/>
+      <c r="AD31" s="17"/>
+      <c r="AE31" s="17"/>
+      <c r="AF31" s="17"/>
+      <c r="AG31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="16" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -2124,13 +2215,15 @@
       <c r="N32" s="17"/>
       <c r="O32" s="17"/>
       <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
+      <c r="Q32" s="38"/>
       <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
+      <c r="S32" s="38"/>
       <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
-      <c r="V32" s="17"/>
-      <c r="W32" s="17"/>
+      <c r="U32" s="38"/>
+      <c r="V32" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="W32" s="42"/>
       <c r="X32" s="17"/>
       <c r="Y32" s="17"/>
       <c r="Z32" s="17"/>
@@ -2143,7 +2236,9 @@
       <c r="AG32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16"/>
+      <c r="A33" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -2159,13 +2254,13 @@
       <c r="N33" s="17"/>
       <c r="O33" s="17"/>
       <c r="P33" s="17"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="17"/>
-      <c r="T33" s="17"/>
-      <c r="U33" s="17"/>
-      <c r="V33" s="17"/>
-      <c r="W33" s="17"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="48"/>
+      <c r="S33" s="48"/>
+      <c r="T33" s="48"/>
+      <c r="U33" s="48"/>
+      <c r="V33" s="38"/>
+      <c r="W33" s="38"/>
       <c r="X33" s="17"/>
       <c r="Y33" s="17"/>
       <c r="Z33" s="17"/>
@@ -2178,45 +2273,45 @@
       <c r="AG33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="25"/>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="25"/>
-      <c r="S34" s="25"/>
-      <c r="T34" s="25"/>
-      <c r="U34" s="25"/>
-      <c r="V34" s="25"/>
-      <c r="W34" s="25"/>
-      <c r="X34" s="25"/>
-      <c r="Y34" s="25"/>
-      <c r="Z34" s="25"/>
-      <c r="AA34" s="25"/>
-      <c r="AB34" s="25"/>
-      <c r="AC34" s="25"/>
-      <c r="AD34" s="25"/>
-      <c r="AE34" s="25"/>
-      <c r="AF34" s="25"/>
-      <c r="AG34" s="26"/>
+      <c r="A34" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="48"/>
+      <c r="R34" s="48"/>
+      <c r="S34" s="48"/>
+      <c r="T34" s="48"/>
+      <c r="U34" s="48"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="42"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="17"/>
+      <c r="AD34" s="17"/>
+      <c r="AE34" s="17"/>
+      <c r="AF34" s="17"/>
+      <c r="AG34" s="19"/>
     </row>
     <row r="35" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -2233,13 +2328,13 @@
       <c r="N35" s="17"/>
       <c r="O35" s="17"/>
       <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="17"/>
-      <c r="T35" s="17"/>
-      <c r="U35" s="17"/>
-      <c r="V35" s="17"/>
-      <c r="W35" s="17"/>
+      <c r="Q35" s="48"/>
+      <c r="R35" s="48"/>
+      <c r="S35" s="48"/>
+      <c r="T35" s="48"/>
+      <c r="U35" s="48"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="44"/>
       <c r="X35" s="17"/>
       <c r="Y35" s="17"/>
       <c r="Z35" s="17"/>
@@ -2252,9 +2347,7 @@
       <c r="AG35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16" t="s">
-        <v>54</v>
-      </c>
+      <c r="A36" s="16"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
@@ -2288,46 +2381,46 @@
       <c r="AF36" s="17"/>
       <c r="AG36" s="19"/>
     </row>
-    <row r="37" customFormat="false" ht="20.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="17"/>
-      <c r="T37" s="17"/>
-      <c r="U37" s="17"/>
-      <c r="V37" s="17"/>
-      <c r="W37" s="17"/>
-      <c r="X37" s="17"/>
-      <c r="Y37" s="17"/>
-      <c r="Z37" s="17"/>
-      <c r="AA37" s="17"/>
-      <c r="AB37" s="17"/>
-      <c r="AC37" s="17"/>
-      <c r="AD37" s="17"/>
-      <c r="AE37" s="17"/>
-      <c r="AF37" s="17"/>
-      <c r="AG37" s="19"/>
-    </row>
-    <row r="38" customFormat="false" ht="20.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="14"/>
+      <c r="AF37" s="14"/>
+      <c r="AG37" s="15"/>
+    </row>
+    <row r="38" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -2361,6 +2454,226 @@
       <c r="AE38" s="17"/>
       <c r="AF38" s="17"/>
       <c r="AG38" s="19"/>
+    </row>
+    <row r="39" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
+      <c r="Y39" s="17"/>
+      <c r="Z39" s="17"/>
+      <c r="AA39" s="17"/>
+      <c r="AB39" s="17"/>
+      <c r="AC39" s="17"/>
+      <c r="AD39" s="17"/>
+      <c r="AE39" s="17"/>
+      <c r="AF39" s="17"/>
+      <c r="AG39" s="19"/>
+    </row>
+    <row r="40" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="25"/>
+      <c r="S40" s="25"/>
+      <c r="T40" s="25"/>
+      <c r="U40" s="25"/>
+      <c r="V40" s="25"/>
+      <c r="W40" s="25"/>
+      <c r="X40" s="25"/>
+      <c r="Y40" s="25"/>
+      <c r="Z40" s="25"/>
+      <c r="AA40" s="25"/>
+      <c r="AB40" s="25"/>
+      <c r="AC40" s="25"/>
+      <c r="AD40" s="25"/>
+      <c r="AE40" s="25"/>
+      <c r="AF40" s="25"/>
+      <c r="AG40" s="26"/>
+    </row>
+    <row r="41" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="17"/>
+      <c r="U41" s="17"/>
+      <c r="V41" s="17"/>
+      <c r="W41" s="17"/>
+      <c r="X41" s="17"/>
+      <c r="Y41" s="17"/>
+      <c r="Z41" s="17"/>
+      <c r="AA41" s="17"/>
+      <c r="AB41" s="17"/>
+      <c r="AC41" s="17"/>
+      <c r="AD41" s="17"/>
+      <c r="AE41" s="17"/>
+      <c r="AF41" s="17"/>
+      <c r="AG41" s="19"/>
+    </row>
+    <row r="42" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="17"/>
+      <c r="Z42" s="17"/>
+      <c r="AA42" s="17"/>
+      <c r="AB42" s="17"/>
+      <c r="AC42" s="17"/>
+      <c r="AD42" s="17"/>
+      <c r="AE42" s="17"/>
+      <c r="AF42" s="17"/>
+      <c r="AG42" s="19"/>
+    </row>
+    <row r="43" customFormat="false" ht="20.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+      <c r="Q43" s="17"/>
+      <c r="R43" s="17"/>
+      <c r="S43" s="17"/>
+      <c r="T43" s="17"/>
+      <c r="U43" s="17"/>
+      <c r="V43" s="17"/>
+      <c r="W43" s="17"/>
+      <c r="X43" s="17"/>
+      <c r="Y43" s="17"/>
+      <c r="Z43" s="17"/>
+      <c r="AA43" s="17"/>
+      <c r="AB43" s="17"/>
+      <c r="AC43" s="17"/>
+      <c r="AD43" s="17"/>
+      <c r="AE43" s="17"/>
+      <c r="AF43" s="17"/>
+      <c r="AG43" s="19"/>
+    </row>
+    <row r="44" customFormat="false" ht="20.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="17"/>
+      <c r="Y44" s="17"/>
+      <c r="Z44" s="17"/>
+      <c r="AA44" s="17"/>
+      <c r="AB44" s="17"/>
+      <c r="AC44" s="17"/>
+      <c r="AD44" s="17"/>
+      <c r="AE44" s="17"/>
+      <c r="AF44" s="17"/>
+      <c r="AG44" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -2405,9 +2718,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.61395348837209"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>